<commit_message>
Major cleanup and improvements: Remove unused Assets component, clean up temporary files, update Plant page with progress tracking and improved UI, fix template codes and frequencies, update README with current features
</commit_message>
<xml_diff>
--- a/server/Inventory list/Inventory Count.xlsx
+++ b/server/Inventory list/Inventory Count.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Inventory " state="visible" r:id="rId4"/>
@@ -5395,18 +5395,18 @@
   <dimension ref="A1:L317"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="J251" sqref="J251"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="1" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5440,7 +5440,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" ht="13.8" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" ht="13.9" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5743,7 +5743,7 @@
         <v>9</v>
       </c>
       <c r="F21" s="17">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" ht="12" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5891,16 +5891,12 @@
       <c r="F30" s="13"/>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
-        <v>0</v>
-      </c>
+      <c r="A31" s="19"/>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
-      <c r="F31" s="10">
-        <v>0</v>
-      </c>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" ht="12" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
@@ -6806,7 +6802,7 @@
       <c r="E83" s="13"/>
       <c r="F83" s="16"/>
     </row>
-    <row r="84" ht="23.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" ht="23.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="23"/>
       <c r="B84" s="23"/>
       <c r="C84" s="23"/>
@@ -6824,7 +6820,7 @@
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
         <v>44</v>
       </c>
@@ -7180,7 +7176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="10">
         <v>280</v>
       </c>
@@ -7210,7 +7206,7 @@
       <c r="E105" s="13"/>
       <c r="F105" s="16"/>
     </row>
-    <row r="106" ht="18.45" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" ht="18.4" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="23"/>
       <c r="B106" s="23"/>
       <c r="C106" s="23"/>
@@ -7228,7 +7224,7 @@
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
     </row>
-    <row r="108" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
         <v>151</v>
       </c>
@@ -7496,7 +7492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="10">
         <v>207</v>
       </c>
@@ -7524,7 +7520,7 @@
       <c r="E123" s="13"/>
       <c r="F123" s="16"/>
     </row>
-    <row r="124" ht="23.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" ht="23.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="23"/>
       <c r="B124" s="23"/>
       <c r="C124" s="23"/>
@@ -7622,7 +7618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="10">
         <v>149</v>
       </c>
@@ -7652,7 +7648,7 @@
       <c r="E131" s="13"/>
       <c r="F131" s="16"/>
     </row>
-    <row r="132" ht="23.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" ht="23.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="23"/>
       <c r="B132" s="23"/>
       <c r="C132" s="23"/>
@@ -7670,7 +7666,7 @@
       <c r="E133" s="13"/>
       <c r="F133" s="16"/>
     </row>
-    <row r="134" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="18">
         <v>1.1</v>
       </c>
@@ -7710,7 +7706,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="136" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="18">
         <v>1.3</v>
       </c>
@@ -7738,7 +7734,7 @@
       <c r="E137" s="13"/>
       <c r="F137" s="16"/>
     </row>
-    <row r="138" ht="18.45" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" ht="18.4" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="23"/>
       <c r="B138" s="23"/>
       <c r="C138" s="23"/>
@@ -7756,7 +7752,7 @@
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
     </row>
-    <row r="140" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="10">
         <v>13</v>
       </c>
@@ -8916,7 +8912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="10">
         <v>215</v>
       </c>
@@ -8944,7 +8940,7 @@
       <c r="E200" s="13"/>
       <c r="F200" s="16"/>
     </row>
-    <row r="201" ht="23.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" ht="23.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="23"/>
       <c r="B201" s="23"/>
       <c r="C201" s="23"/>
@@ -8962,7 +8958,7 @@
       <c r="E202" s="5"/>
       <c r="F202" s="5"/>
     </row>
-    <row r="203" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="10">
         <v>6</v>
       </c>
@@ -9162,7 +9158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="10">
         <v>303</v>
       </c>
@@ -9190,7 +9186,7 @@
       <c r="E214" s="13"/>
       <c r="F214" s="16"/>
     </row>
-    <row r="215" ht="17.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" ht="17.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="23"/>
       <c r="B215" s="23"/>
       <c r="C215" s="23"/>
@@ -9208,7 +9204,7 @@
       <c r="E216" s="13"/>
       <c r="F216" s="16"/>
     </row>
-    <row r="217" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="10">
         <v>114</v>
       </c>
@@ -9528,7 +9524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="10">
         <v>188</v>
       </c>
@@ -9556,7 +9552,7 @@
       <c r="E234" s="13"/>
       <c r="F234" s="16"/>
     </row>
-    <row r="235" ht="18.45" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" ht="18.4" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="23"/>
       <c r="B235" s="23"/>
       <c r="C235" s="23"/>
@@ -9574,7 +9570,7 @@
       <c r="E236" s="5"/>
       <c r="F236" s="5"/>
     </row>
-    <row r="237" ht="13.95" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" ht="13.9" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="10">
         <v>66</v>
       </c>
@@ -9932,7 +9928,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="254" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="25" t="s">
         <v>395</v>
       </c>
@@ -9962,7 +9958,7 @@
       <c r="E255" s="13"/>
       <c r="F255" s="16"/>
     </row>
-    <row r="256" ht="23.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" ht="23.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="23"/>
       <c r="B256" s="23"/>
       <c r="C256" s="23"/>
@@ -9980,7 +9976,7 @@
       <c r="E257" s="13"/>
       <c r="F257" s="16"/>
     </row>
-    <row r="258" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="10">
         <v>87</v>
       </c>
@@ -10264,7 +10260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="18">
         <v>107.4</v>
       </c>
@@ -10292,7 +10288,7 @@
       <c r="E273" s="13"/>
       <c r="F273" s="16"/>
     </row>
-    <row r="274" ht="18.45" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" ht="18.4" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="23"/>
       <c r="B274" s="23"/>
       <c r="C274" s="23"/>
@@ -10310,7 +10306,7 @@
       <c r="E275" s="13"/>
       <c r="F275" s="16"/>
     </row>
-    <row r="276" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="10">
         <v>108</v>
       </c>
@@ -10390,7 +10386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="10">
         <v>112</v>
       </c>
@@ -10420,7 +10416,7 @@
       <c r="E281" s="13"/>
       <c r="F281" s="16"/>
     </row>
-    <row r="282" ht="23.55" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" ht="23.65" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="23"/>
       <c r="B282" s="23"/>
       <c r="C282" s="23"/>
@@ -10438,7 +10434,7 @@
       <c r="E283" s="5"/>
       <c r="F283" s="5"/>
     </row>
-    <row r="284" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="10">
         <v>250</v>
       </c>
@@ -10746,7 +10742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="10">
         <v>365</v>
       </c>
@@ -10784,7 +10780,7 @@
       <c r="E303" s="5"/>
       <c r="F303" s="5"/>
     </row>
-    <row r="304" ht="13.05" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" ht="13.15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="10">
         <v>300</v>
       </c>
@@ -10994,7 +10990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" ht="13.95" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" ht="13.9" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="10">
         <v>5</v>
       </c>

</xml_diff>